<commit_message>
minor changes more to come
</commit_message>
<xml_diff>
--- a/Documents/Week6/06_Team3WorkRequestRequirementsTraceabilityMatrixTemplate.xlsx
+++ b/Documents/Week6/06_Team3WorkRequestRequirementsTraceabilityMatrixTemplate.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\Documents\GitHub\UMGC_495_7381_Work_Request\Documents\Week5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepo\Documents\Week6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED26C9A6-DD8E-4A68-94FC-A61A03D5C614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85572480-AEC1-4E26-9880-2FB0B7F46C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Traceability Template'!$A$1:$J$34</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
   <si>
     <t>Project Name</t>
   </si>
@@ -199,6 +200,9 @@
   </si>
   <si>
     <t>Requested by</t>
+  </si>
+  <si>
+    <t>Discontinued</t>
   </si>
 </sst>
 </file>
@@ -257,7 +261,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +310,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -475,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -522,6 +532,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -529,6 +548,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -542,9 +564,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -890,8 +909,8 @@
   </sheetPr>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -909,80 +928,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="16"/>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="14"/>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="27" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="14"/>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="18" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="28">
+      <c r="F4" s="27"/>
+      <c r="G4" s="26">
         <v>44544</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" ht="26.25" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
@@ -1035,7 +1054,9 @@
       <c r="F6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H6" s="3" t="s">
         <v>52</v>
       </c>
@@ -1065,7 +1086,9 @@
       <c r="F7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1077,32 +1100,34 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="3">
+      <c r="I8" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="19">
         <v>1003</v>
       </c>
     </row>
@@ -1125,7 +1150,9 @@
       <c r="F9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>52</v>
       </c>
@@ -1155,9 +1182,11 @@
       <c r="F10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H10" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>40</v>
@@ -1185,7 +1214,9 @@
       <c r="F11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H11" s="3" t="s">
         <v>54</v>
       </c>
@@ -1215,9 +1246,11 @@
       <c r="F12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H12" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>53</v>
@@ -1245,7 +1278,9 @@
       <c r="F13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>54</v>
       </c>
@@ -2177,4 +2212,16 @@
     <oddFooter>&amp;L&amp;9© 2009 Regents of the University of Minnesota. All rights reserved.&amp;R&amp;9Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D356D46-0B48-4462-9928-DD6A8ADBC5D6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>